<commit_message>
Changes with respect to adding in test modules loop
</commit_message>
<xml_diff>
--- a/LearnMetTestAutomation/src/main/resources/InputSheet1.xlsx
+++ b/LearnMetTestAutomation/src/main/resources/InputSheet1.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LearnMetAutomationWorkspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prita\git\LearnMetTestAutomation\LearnMetTestAutomation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4261E628-4389-4A41-9B11-EAB39788A4BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCB57EE-5BBA-4F47-AEB5-0838E5DCA062}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D86B3A5-D981-4A3B-9E22-0DFE7341FA21}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="2" xr2:uid="{7D86B3A5-D981-4A3B-9E22-0DFE7341FA21}"/>
   </bookViews>
   <sheets>
-    <sheet name="GoogleTest" sheetId="1" r:id="rId1"/>
+    <sheet name="TestModules" sheetId="3" r:id="rId1"/>
+    <sheet name="GoogleTest" sheetId="1" r:id="rId2"/>
+    <sheet name="CourseCreation" sheetId="2" r:id="rId3"/>
+    <sheet name="CourseModification" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>Test Step No.</t>
   </si>
@@ -88,13 +91,58 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>(//a[@class='dropdown-toggle'])[2]//following::li[7]/a/div</t>
+  </si>
+  <si>
+    <t>Click on the Sign In Page</t>
+  </si>
+  <si>
+    <t>//input[@name='j_username']</t>
+  </si>
+  <si>
+    <t>Enter Username</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Enter Password</t>
+  </si>
+  <si>
+    <t>//input[@name='j_password']</t>
+  </si>
+  <si>
+    <t>learnmet</t>
+  </si>
+  <si>
+    <t>Le@rnmet</t>
+  </si>
+  <si>
+    <t>//input[@name='j_passord']</t>
+  </si>
+  <si>
+    <t>ModuleName</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>CourseCreation</t>
+  </si>
+  <si>
+    <t>CourseModification</t>
+  </si>
+  <si>
+    <t>5000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,8 +157,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,11 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,11 +516,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31189D19-4FE9-4043-80D3-938F5BFC5FF1}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC454C21-2CE3-4050-85B4-7903E8DA7D76}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:AM3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,4 +648,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D804BB-CF41-46BF-B6A6-6C1008107EE7}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9494385-0BC6-445A-8685-28DEC0B1EB6D}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes with respect to addtion Dropdown Select function Changes with respect to Course creation inputsheet (adding test steps)
</commit_message>
<xml_diff>
--- a/LearnMetTestAutomation/src/main/resources/InputSheet1.xlsx
+++ b/LearnMetTestAutomation/src/main/resources/InputSheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prita\git\LearnMetTestAutomation\LearnMetTestAutomation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCB57EE-5BBA-4F47-AEB5-0838E5DCA062}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60BEEC-05F4-49BA-9843-FAB9B33FF9B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="2" xr2:uid="{7D86B3A5-D981-4A3B-9E22-0DFE7341FA21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7D86B3A5-D981-4A3B-9E22-0DFE7341FA21}"/>
   </bookViews>
   <sheets>
     <sheet name="TestModules" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="199">
   <si>
     <t>Test Step No.</t>
   </si>
@@ -132,10 +132,505 @@
     <t>CourseCreation</t>
   </si>
   <si>
-    <t>CourseModification</t>
-  </si>
-  <si>
     <t>5000</t>
+  </si>
+  <si>
+    <t>sohom.qa@gmail.com</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>//button[@type='submit']</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Click on Login Button</t>
+  </si>
+  <si>
+    <t>//a[@class='btn btn-control bg-blue']</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Click on my DashBoard</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>//i[@class='fa fa fa-random']/following::b[1]</t>
+  </si>
+  <si>
+    <t>Click on Switch Teacher Mode</t>
+  </si>
+  <si>
+    <t>//span[text()='Course']</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Click on Course Tab</t>
+  </si>
+  <si>
+    <t>//ul[@id='course-menu']/li</t>
+  </si>
+  <si>
+    <t>DropdownSelect</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Select Dropdown</t>
+  </si>
+  <si>
+    <t>Create New Course</t>
+  </si>
+  <si>
+    <t>MoveToElement&amp;Click</t>
+  </si>
+  <si>
+    <t>//span[text()='Recordings']</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Move down to tab create course</t>
+  </si>
+  <si>
+    <t>MoveToElement</t>
+  </si>
+  <si>
+    <t>courseTitle</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>idSendkey</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Write Course Title</t>
+  </si>
+  <si>
+    <t>Selenium Advance Course</t>
+  </si>
+  <si>
+    <t>smallDesc</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Write Short Description</t>
+  </si>
+  <si>
+    <t>This Course is intended to help gaining industrial knowledge with practical case studies</t>
+  </si>
+  <si>
+    <t>contentDesc</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Write Course Summary</t>
+  </si>
+  <si>
+    <t>countryId</t>
+  </si>
+  <si>
+    <t>idDropdownSelect</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Select country from dropdown</t>
+  </si>
+  <si>
+    <t>Global(ALL)</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Select course lang from dropdown</t>
+  </si>
+  <si>
+    <t>languageId</t>
+  </si>
+  <si>
+    <t>learnGrpId</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Select learning grp from dropdown</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>Select learning level from dropdown</t>
+  </si>
+  <si>
+    <t>(//*[@id='learnlvlId'])[1]</t>
+  </si>
+  <si>
+    <t>(//*[@id='learnlvlId'])[2]</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Select learning stage from dropdown</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>xpathDropdownSelect</t>
+  </si>
+  <si>
+    <t>courseDlvryId</t>
+  </si>
+  <si>
+    <t>Self Study</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Select course delivery from dropdown</t>
+  </si>
+  <si>
+    <t>(//i[@class='md md-edit'])[1]</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Switch to Chapter1 Section1</t>
+  </si>
+  <si>
+    <t>Click on Chapter1 Section1</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>//iframe[@class='cke_wysiwyg_frame cke_reset']</t>
+  </si>
+  <si>
+    <t>SwitchToIframe</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Write to Chapter1 Section1</t>
+  </si>
+  <si>
+    <t>//body[contains(@class,'cke_editable_themed cke_contents_ltr')]</t>
+  </si>
+  <si>
+    <t>Welcome to Chapter1 Section1</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Switch Back to normal mode</t>
+  </si>
+  <si>
+    <t>SwitchToDefault</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>DurationHrs</t>
+  </si>
+  <si>
+    <t>DurationMin</t>
+  </si>
+  <si>
+    <t>Set Chapter hour Duration</t>
+  </si>
+  <si>
+    <t>Set Chapter minute Duration</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>//button[@class='swal2-confirm styled']</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Click on Submit Button</t>
+  </si>
+  <si>
+    <t>Click on OK Button</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>(//i[@class='md md-edit'])[5]</t>
+  </si>
+  <si>
+    <t>Move to last Chapter</t>
+  </si>
+  <si>
+    <t>(//i[@class='md md-edit'])[2]</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>(//i[@class='md md-edit'])[3]</t>
+  </si>
+  <si>
+    <t>Welcome to Chapter1 Section3</t>
+  </si>
+  <si>
+    <t>Welcome to Chapter1 Section2</t>
+  </si>
+  <si>
+    <t>Click on Chapter1 Section3</t>
+  </si>
+  <si>
+    <t>Switch to Chapter1 Section3</t>
+  </si>
+  <si>
+    <t>Write to Chapter1 Section3</t>
+  </si>
+  <si>
+    <t>Click on Chapter1 Section2</t>
+  </si>
+  <si>
+    <t>Switch to Chapter1 Section2</t>
+  </si>
+  <si>
+    <t>Write to Chapter1 Section2</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>Click on Chapter1 Section4</t>
+  </si>
+  <si>
+    <t>Switch to Chapter1 Section4</t>
+  </si>
+  <si>
+    <t>Write to Chapter1 Section4</t>
+  </si>
+  <si>
+    <t>(//i[@class='md md-edit'])[4]</t>
+  </si>
+  <si>
+    <t>Welcome to Chapter1 Section4</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Click on Chapter1 Section5</t>
+  </si>
+  <si>
+    <t>Switch to Chapter1 Section5</t>
+  </si>
+  <si>
+    <t>Write to Chapter1 Section5</t>
+  </si>
+  <si>
+    <t>Welcome to Chapter1 Section5</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>(//a[@title='Delete Chapter'])[2]</t>
+  </si>
+  <si>
+    <t>Click on delete Chapter</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>Click on Confirm Delete</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>Click on Save Course</t>
+  </si>
+  <si>
+    <t>//*[@id='saveCourseNew']</t>
+  </si>
+  <si>
+    <t>7000</t>
+  </si>
+  <si>
+    <t>(//p[@class='text-subhead text-light'])[1]//span[1]//i</t>
+  </si>
+  <si>
+    <t>//a[@title='All/Public']</t>
+  </si>
+  <si>
+    <t>//a[@id='viewAsset368']/following::a[1]</t>
+  </si>
+  <si>
+    <t>Click on pic/video Upload Link</t>
+  </si>
+  <si>
+    <t>Click on public folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on image </t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>courseVisibility</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Select visibility from dropdown</t>
+  </si>
+  <si>
+    <t>66</t>
   </si>
 </sst>
 </file>
@@ -196,13 +691,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31189D19-4FE9-4043-80D3-938F5BFC5FF1}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,14 +1048,6 @@
       </c>
       <c r="B2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -652,17 +1149,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D804BB-CF41-46BF-B6A6-6C1008107EE7}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -727,8 +1225,8 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>26</v>
+      <c r="F3" t="s">
+        <v>33</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
@@ -750,15 +1248,1457 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>27</v>
+      <c r="F4" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>59</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B55" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" t="s">
+        <v>59</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" t="s">
+        <v>177</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" t="s">
+        <v>189</v>
+      </c>
+      <c r="C64" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>